<commit_message>
Converts BCoESC to a time-series variable per US-copy branch (not properly merged)
</commit_message>
<xml_diff>
--- a/InputData/elec/BCoESC/BAU Cost of Electricity Sector Capital.xlsx
+++ b/InputData/elec/BCoESC/BAU Cost of Electricity Sector Capital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Francis Swint\Vensim\eps-eu\InputData\elec\BCoESC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\elec\BCoESC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC410CF-3F6D-47B0-9AB2-AFA0E137AA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE3F036-1CF0-47D7-934A-6B4F4C83C54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="3" xr2:uid="{752771AD-C619-44A2-86AD-40FE48642E30}"/>
+    <workbookView xWindow="31080" yWindow="2295" windowWidth="26310" windowHeight="14610" activeTab="3" xr2:uid="{752771AD-C619-44A2-86AD-40FE48642E30}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>BAU BCoESC Cost of Electricity Sector Capital for Power Plants</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Unit: dimensionless (% of project cost)</t>
-  </si>
-  <si>
-    <t>cost of financing</t>
   </si>
   <si>
     <t>hard coal</t>
@@ -281,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -292,9 +289,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -484,9 +478,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -524,7 +518,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -630,7 +624,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -772,7 +766,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -909,20 +903,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA929DFA-FED7-428C-BCB6-8D6BF5DF7845}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="54" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
@@ -939,11 +933,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -959,10 +953,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,226 +965,3097 @@
     <col min="2" max="2" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="B2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="B3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE3" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+      <c r="B4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE4" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="B5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE5" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="B6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE6" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="B7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE7" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE8" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="B9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE9" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="B10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE10" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+      <c r="B11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE11" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="11" t="s">
+      <c r="B12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE12" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="B13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE13" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="B14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE14" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="B15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE15" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="B16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE16" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="B17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE17" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+      <c r="B18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE18" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE19" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE20" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE21" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+      <c r="B22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE22" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+      <c r="B23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE23" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
+      <c r="B24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE24" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="11">
-        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD25" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE25" s="10">
         <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
         <v>0.08</v>
       </c>
@@ -1205,10 +4070,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1217,19 +4082,222 @@
     <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="11">
+      <c r="B1">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="C2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="D2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="E2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="F2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="G2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="H2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="I2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="J2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="K2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="L2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="M2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="N2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="O2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="P2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Q2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="R2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="S2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="T2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="U2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="V2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="W2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="X2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Y2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="Z2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AA2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AB2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AC2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AD2" s="10">
+        <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
+        <v>0.08</v>
+      </c>
+      <c r="AE2" s="10">
         <f>'WACC data'!$C$24-'WACC data'!$B$29/100</f>
         <v>0.08</v>
       </c>
@@ -1240,6 +4308,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
     <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
@@ -1462,27 +4550,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1416CD70-5DE9-4BBA-85C9-91780834DFBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B805194B-003B-4534-A283-55F3425DA64D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C757C7E-C121-410A-952C-CAF9644A33D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1499,23 +4586,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B805194B-003B-4534-A283-55F3425DA64D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1416CD70-5DE9-4BBA-85C9-91780834DFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>